<commit_message>
almost done except rewriting new clients over old clients
</commit_message>
<xml_diff>
--- a/ProjetTp2/Clients.xlsx
+++ b/ProjetTp2/Clients.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\A\B43Officiel\tps\TP2\RemettreEtudiants+Enoncé\ProjetTp2\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="44">
   <si>
     <t>Numéro de carte</t>
   </si>
@@ -93,13 +93,74 @@
   </si>
   <si>
     <t>Charles Bouvier Dondo</t>
+  </si>
+  <si>
+    <t>222444</t>
+  </si>
+  <si>
+    <t>330978</t>
+  </si>
+  <si>
+    <t>777666</t>
+  </si>
+  <si>
+    <t>222222</t>
+  </si>
+  <si>
+    <t>558844</t>
+  </si>
+  <si>
+    <t>222999</t>
+  </si>
+  <si>
+    <t>111222</t>
+  </si>
+  <si>
+    <t>302233</t>
+  </si>
+  <si>
+    <t>222000</t>
+  </si>
+  <si>
+    <t>111888</t>
+  </si>
+  <si>
+    <t>333666</t>
+  </si>
+  <si>
+    <t>444555</t>
+  </si>
+  <si>
+    <t>555444</t>
+  </si>
+  <si>
+    <t>123123</t>
+  </si>
+  <si>
+    <t>252525</t>
+  </si>
+  <si>
+    <t>888999</t>
+  </si>
+  <si>
+    <t>333555</t>
+  </si>
+  <si>
+    <t>112233</t>
+  </si>
+  <si>
+    <t>999777</t>
+  </si>
+  <si>
+    <t>996644</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,9 +504,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="45.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -463,283 +524,283 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>111888</v>
+      <c r="A2" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>40</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="C2" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>222222</v>
+      <c r="A3" t="s">
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>130</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="C3" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>111222</v>
+      <c r="A4" t="s">
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>250</v>
-      </c>
-      <c r="D4">
-        <v>45.9</v>
+        <v>16</v>
+      </c>
+      <c r="C4" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>302233</v>
+      <c r="A5" t="s">
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>1234.8900000000001</v>
+        <v>16</v>
+      </c>
+      <c r="C5" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>777666</v>
+      <c r="A6" t="s">
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>500</v>
-      </c>
-      <c r="D6">
-        <v>1234.9000000000001</v>
+        <v>16</v>
+      </c>
+      <c r="C6" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>333666</v>
+      <c r="A7" t="s">
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>710</v>
-      </c>
-      <c r="D7">
-        <v>34.369999999999997</v>
+        <v>16</v>
+      </c>
+      <c r="C7" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>330978</v>
+      <c r="A8" t="s">
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>458.99</v>
+        <v>16</v>
+      </c>
+      <c r="C8" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>222000</v>
+      <c r="A9" t="s">
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>975</v>
-      </c>
-      <c r="D9">
-        <v>12.65</v>
+        <v>16</v>
+      </c>
+      <c r="C9" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>444555</v>
+      <c r="A10" t="s">
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>260</v>
-      </c>
-      <c r="D10">
-        <v>400.09</v>
+        <v>16</v>
+      </c>
+      <c r="C10" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>112233</v>
+      <c r="A11" t="s">
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>1890.34</v>
+        <v>16</v>
+      </c>
+      <c r="C11" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>333555</v>
+      <c r="A12" t="s">
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>29</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="C12" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>888999</v>
+      <c r="A13" t="s">
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>778</v>
-      </c>
-      <c r="D13">
-        <v>310.39999999999998</v>
+        <v>16</v>
+      </c>
+      <c r="C13" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>996644</v>
+      <c r="A14" t="s">
+        <v>43</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C14">
-        <v>140</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
+      <c r="C14" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>558844</v>
+      <c r="A15" t="s">
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15">
-        <v>15</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="C15" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>222444</v>
+      <c r="A16" t="s">
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16">
-        <v>100</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="C16" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>222999</v>
+      <c r="A17" t="s">
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="C17" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>999777</v>
+      <c r="A18" t="s">
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18">
-        <v>120</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="C18" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>555444</v>
+      <c r="A19" t="s">
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19">
-        <v>200</v>
-      </c>
-      <c r="D19">
-        <v>120</v>
+        <v>16</v>
+      </c>
+      <c r="C19" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>252525</v>
+      <c r="A20" t="s">
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20">
-        <v>500</v>
-      </c>
-      <c r="D20">
-        <v>250</v>
+        <v>16</v>
+      </c>
+      <c r="C20" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>123123</v>
+      <c r="A21" t="s">
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21">
-        <v>450</v>
-      </c>
-      <c r="D21">
-        <v>350</v>
+        <v>16</v>
+      </c>
+      <c r="C21" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
done! - missing comments
</commit_message>
<xml_diff>
--- a/ProjetTp2/Clients.xlsx
+++ b/ProjetTp2/Clients.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\A\B43Officiel\tps\TP2\RemettreEtudiants+Enoncé\ProjetTp2\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Numéro de carte</t>
   </si>
@@ -93,74 +93,13 @@
   </si>
   <si>
     <t>Charles Bouvier Dondo</t>
-  </si>
-  <si>
-    <t>222444</t>
-  </si>
-  <si>
-    <t>330978</t>
-  </si>
-  <si>
-    <t>777666</t>
-  </si>
-  <si>
-    <t>222222</t>
-  </si>
-  <si>
-    <t>558844</t>
-  </si>
-  <si>
-    <t>222999</t>
-  </si>
-  <si>
-    <t>111222</t>
-  </si>
-  <si>
-    <t>302233</t>
-  </si>
-  <si>
-    <t>222000</t>
-  </si>
-  <si>
-    <t>111888</t>
-  </si>
-  <si>
-    <t>333666</t>
-  </si>
-  <si>
-    <t>444555</t>
-  </si>
-  <si>
-    <t>555444</t>
-  </si>
-  <si>
-    <t>123123</t>
-  </si>
-  <si>
-    <t>252525</t>
-  </si>
-  <si>
-    <t>888999</t>
-  </si>
-  <si>
-    <t>333555</t>
-  </si>
-  <si>
-    <t>112233</t>
-  </si>
-  <si>
-    <t>999777</t>
-  </si>
-  <si>
-    <t>996644</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,9 +443,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="45.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="1" max="2" width="27.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -524,283 +463,283 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>43</v>
+      <c r="A2" s="1">
+        <v>111888</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.0</v>
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>43</v>
+      <c r="A3">
+        <v>222222</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.0</v>
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>130</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>43</v>
+      <c r="A4">
+        <v>111222</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.0</v>
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>250</v>
+      </c>
+      <c r="D4">
+        <v>45.9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>43</v>
+      <c r="A5">
+        <v>302233</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.0</v>
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1234.8900000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>43</v>
+      <c r="A6">
+        <v>777666</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.0</v>
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>500</v>
+      </c>
+      <c r="D6">
+        <v>1234.9000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>43</v>
+      <c r="A7">
+        <v>333666</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.0</v>
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>710</v>
+      </c>
+      <c r="D7">
+        <v>34.369999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>43</v>
+      <c r="A8">
+        <v>330978</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.0</v>
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>458.99</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
+      <c r="A9">
+        <v>222000</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.0</v>
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>975</v>
+      </c>
+      <c r="D9">
+        <v>12.65</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>43</v>
+      <c r="A10">
+        <v>444555</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.0</v>
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>260</v>
+      </c>
+      <c r="D10">
+        <v>400.09</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
+      <c r="A11">
+        <v>112233</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.0</v>
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1890.34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>43</v>
+      <c r="A12">
+        <v>333555</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.0</v>
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>43</v>
+      <c r="A13">
+        <v>888999</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.0</v>
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>778</v>
+      </c>
+      <c r="D13">
+        <v>310.39999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>43</v>
+      <c r="A14">
+        <v>996644</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.0</v>
+      <c r="C14">
+        <v>140</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>43</v>
+      <c r="A15">
+        <v>558844</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.0</v>
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>43</v>
+      <c r="A16">
+        <v>222444</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.0</v>
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>43</v>
+      <c r="A17">
+        <v>222999</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.0</v>
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>43</v>
+      <c r="A18">
+        <v>999777</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.0</v>
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>120</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>43</v>
+      <c r="A19">
+        <v>555444</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.0</v>
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>200</v>
+      </c>
+      <c r="D19">
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>43</v>
+      <c r="A20">
+        <v>252525</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0.0</v>
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>500</v>
+      </c>
+      <c r="D20">
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>43</v>
+      <c r="A21">
+        <v>123123</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" t="n">
-        <v>140.0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.0</v>
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>450</v>
+      </c>
+      <c r="D21">
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>